<commit_message>
More appropriate language in examples
</commit_message>
<xml_diff>
--- a/benchmarking/TerrestrialAIM_DataAnalysis_Template.xlsx
+++ b/benchmarking/TerrestrialAIM_DataAnalysis_Template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4070" uniqueCount="1365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4070" uniqueCount="1363">
   <si>
     <t>Management Question</t>
   </si>
@@ -3935,12 +3935,6 @@
   </si>
   <si>
     <t>Marginal</t>
-  </si>
-  <si>
-    <t>Ruined</t>
-  </si>
-  <si>
-    <t>Acceptable</t>
   </si>
   <si>
     <t>Benchmark Source</t>
@@ -5430,6 +5424,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="7" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5459,18 +5465,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5651,11 +5645,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="70"/>
-        <c:axId val="46926336"/>
-        <c:axId val="46489600"/>
+        <c:axId val="118190080"/>
+        <c:axId val="60707328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="46926336"/>
+        <c:axId val="118190080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5677,7 +5671,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
@@ -5693,7 +5686,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46489600"/>
+        <c:crossAx val="60707328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5701,7 +5694,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46489600"/>
+        <c:axId val="60707328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5744,14 +5737,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46926336"/>
+        <c:crossAx val="118190080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5927,11 +5919,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="70"/>
-        <c:axId val="55805952"/>
-        <c:axId val="46491328"/>
+        <c:axId val="69719552"/>
+        <c:axId val="60709056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="55805952"/>
+        <c:axId val="69719552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5953,7 +5945,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
@@ -5969,7 +5960,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46491328"/>
+        <c:crossAx val="60709056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5977,7 +5968,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46491328"/>
+        <c:axId val="60709056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6020,14 +6011,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55805952"/>
+        <c:crossAx val="69719552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8282,148 +8272,148 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="109" t="s">
         <v>1201</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="105"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="109"/>
+      <c r="J1" s="109"/>
+      <c r="K1" s="109"/>
+      <c r="L1" s="109"/>
     </row>
     <row r="2" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="110" t="s">
         <v>1202</v>
       </c>
-      <c r="B2" s="106"/>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
-      <c r="F2" s="106"/>
-      <c r="G2" s="106"/>
-      <c r="H2" s="106"/>
-      <c r="I2" s="106"/>
-      <c r="J2" s="106"/>
-      <c r="K2" s="106"/>
-      <c r="L2" s="106"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="110"/>
+      <c r="H2" s="110"/>
+      <c r="I2" s="110"/>
+      <c r="J2" s="110"/>
+      <c r="K2" s="110"/>
+      <c r="L2" s="110"/>
     </row>
     <row r="3" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="106" t="s">
+      <c r="A3" s="110" t="s">
         <v>1203</v>
       </c>
-      <c r="B3" s="106"/>
-      <c r="C3" s="106"/>
-      <c r="D3" s="106"/>
-      <c r="E3" s="106"/>
-      <c r="F3" s="106"/>
-      <c r="G3" s="106"/>
-      <c r="H3" s="106"/>
-      <c r="I3" s="106"/>
-      <c r="J3" s="106"/>
-      <c r="K3" s="106"/>
-      <c r="L3" s="106"/>
+      <c r="B3" s="110"/>
+      <c r="C3" s="110"/>
+      <c r="D3" s="110"/>
+      <c r="E3" s="110"/>
+      <c r="F3" s="110"/>
+      <c r="G3" s="110"/>
+      <c r="H3" s="110"/>
+      <c r="I3" s="110"/>
+      <c r="J3" s="110"/>
+      <c r="K3" s="110"/>
+      <c r="L3" s="110"/>
     </row>
     <row r="4" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="109" t="s">
+      <c r="A4" s="113" t="s">
         <v>1212</v>
       </c>
-      <c r="B4" s="109"/>
-      <c r="C4" s="109"/>
-      <c r="D4" s="109"/>
-      <c r="E4" s="109"/>
-      <c r="F4" s="109"/>
-      <c r="G4" s="109"/>
-      <c r="H4" s="109"/>
-      <c r="I4" s="109"/>
-      <c r="J4" s="109"/>
-      <c r="K4" s="109"/>
-      <c r="L4" s="109"/>
+      <c r="B4" s="113"/>
+      <c r="C4" s="113"/>
+      <c r="D4" s="113"/>
+      <c r="E4" s="113"/>
+      <c r="F4" s="113"/>
+      <c r="G4" s="113"/>
+      <c r="H4" s="113"/>
+      <c r="I4" s="113"/>
+      <c r="J4" s="113"/>
+      <c r="K4" s="113"/>
+      <c r="L4" s="113"/>
     </row>
     <row r="5" spans="1:12" ht="102.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="108" t="s">
+      <c r="A5" s="112" t="s">
         <v>1214</v>
       </c>
-      <c r="B5" s="108"/>
-      <c r="C5" s="108"/>
-      <c r="D5" s="108"/>
-      <c r="E5" s="108"/>
-      <c r="F5" s="108"/>
-      <c r="G5" s="108"/>
-      <c r="H5" s="108"/>
-      <c r="I5" s="108"/>
-      <c r="J5" s="108"/>
-      <c r="K5" s="108"/>
-      <c r="L5" s="108"/>
+      <c r="B5" s="112"/>
+      <c r="C5" s="112"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
+      <c r="H5" s="112"/>
+      <c r="I5" s="112"/>
+      <c r="J5" s="112"/>
+      <c r="K5" s="112"/>
+      <c r="L5" s="112"/>
     </row>
     <row r="6" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="109" t="s">
+      <c r="A6" s="113" t="s">
         <v>1210</v>
       </c>
-      <c r="B6" s="109"/>
-      <c r="C6" s="109"/>
-      <c r="D6" s="109"/>
-      <c r="E6" s="109"/>
-      <c r="F6" s="109"/>
-      <c r="G6" s="109"/>
-      <c r="H6" s="109"/>
-      <c r="I6" s="109"/>
-      <c r="J6" s="109"/>
-      <c r="K6" s="109"/>
-      <c r="L6" s="109"/>
+      <c r="B6" s="113"/>
+      <c r="C6" s="113"/>
+      <c r="D6" s="113"/>
+      <c r="E6" s="113"/>
+      <c r="F6" s="113"/>
+      <c r="G6" s="113"/>
+      <c r="H6" s="113"/>
+      <c r="I6" s="113"/>
+      <c r="J6" s="113"/>
+      <c r="K6" s="113"/>
+      <c r="L6" s="113"/>
     </row>
     <row r="7" spans="1:12" ht="161.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="110" t="s">
+      <c r="A7" s="114" t="s">
         <v>1213</v>
       </c>
-      <c r="B7" s="110"/>
-      <c r="C7" s="110"/>
-      <c r="D7" s="110"/>
-      <c r="E7" s="110"/>
-      <c r="F7" s="110"/>
-      <c r="G7" s="110"/>
-      <c r="H7" s="110"/>
-      <c r="I7" s="110"/>
-      <c r="J7" s="110"/>
-      <c r="K7" s="110"/>
-      <c r="L7" s="110"/>
+      <c r="B7" s="114"/>
+      <c r="C7" s="114"/>
+      <c r="D7" s="114"/>
+      <c r="E7" s="114"/>
+      <c r="F7" s="114"/>
+      <c r="G7" s="114"/>
+      <c r="H7" s="114"/>
+      <c r="I7" s="114"/>
+      <c r="J7" s="114"/>
+      <c r="K7" s="114"/>
+      <c r="L7" s="114"/>
     </row>
     <row r="8" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="109" t="s">
+      <c r="A8" s="113" t="s">
         <v>1211</v>
       </c>
-      <c r="B8" s="109"/>
-      <c r="C8" s="109"/>
-      <c r="D8" s="109"/>
-      <c r="E8" s="109"/>
-      <c r="F8" s="109"/>
-      <c r="G8" s="109"/>
-      <c r="H8" s="109"/>
-      <c r="I8" s="109"/>
-      <c r="J8" s="109"/>
-      <c r="K8" s="109"/>
-      <c r="L8" s="109"/>
+      <c r="B8" s="113"/>
+      <c r="C8" s="113"/>
+      <c r="D8" s="113"/>
+      <c r="E8" s="113"/>
+      <c r="F8" s="113"/>
+      <c r="G8" s="113"/>
+      <c r="H8" s="113"/>
+      <c r="I8" s="113"/>
+      <c r="J8" s="113"/>
+      <c r="K8" s="113"/>
+      <c r="L8" s="113"/>
     </row>
     <row r="9" spans="1:12" ht="99" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="107" t="s">
+      <c r="A9" s="111" t="s">
         <v>1209</v>
       </c>
-      <c r="B9" s="107"/>
-      <c r="C9" s="107"/>
-      <c r="D9" s="107"/>
-      <c r="E9" s="107"/>
-      <c r="F9" s="107"/>
-      <c r="G9" s="107"/>
-      <c r="H9" s="107"/>
-      <c r="I9" s="107"/>
-      <c r="J9" s="107"/>
-      <c r="K9" s="107"/>
-      <c r="L9" s="107"/>
+      <c r="B9" s="111"/>
+      <c r="C9" s="111"/>
+      <c r="D9" s="111"/>
+      <c r="E9" s="111"/>
+      <c r="F9" s="111"/>
+      <c r="G9" s="111"/>
+      <c r="H9" s="111"/>
+      <c r="I9" s="111"/>
+      <c r="J9" s="111"/>
+      <c r="K9" s="111"/>
+      <c r="L9" s="111"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="42"/>
@@ -8530,8 +8520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8559,7 +8549,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="92" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="C1" s="96" t="s">
         <v>1218</v>
@@ -8586,10 +8576,10 @@
         <v>1219</v>
       </c>
       <c r="K1" s="100" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
       <c r="L1" s="93" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
       <c r="M1" s="28"/>
       <c r="N1" s="29"/>
@@ -8630,7 +8620,7 @@
       <c r="J2" s="101" t="s">
         <v>1222</v>
       </c>
-      <c r="K2" s="115" t="s">
+      <c r="K2" s="105" t="s">
         <v>890</v>
       </c>
       <c r="L2" s="56">
@@ -8664,7 +8654,7 @@
         <v>891</v>
       </c>
       <c r="F3" s="37" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="G3" s="38" t="s">
         <v>891</v>
@@ -8678,7 +8668,7 @@
       <c r="J3" s="102" t="s">
         <v>1223</v>
       </c>
-      <c r="K3" s="116" t="s">
+      <c r="K3" s="106" t="s">
         <v>888</v>
       </c>
       <c r="L3" s="40">
@@ -8705,7 +8695,7 @@
         <v>888</v>
       </c>
       <c r="F4" s="37" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="G4" s="38" t="s">
         <v>891</v>
@@ -8719,7 +8709,7 @@
       <c r="J4" s="102" t="s">
         <v>1224</v>
       </c>
-      <c r="K4" s="116"/>
+      <c r="K4" s="106"/>
       <c r="L4" s="40"/>
       <c r="Q4" t="s">
         <v>889</v>
@@ -8745,7 +8735,7 @@
         <v>888</v>
       </c>
       <c r="F5" s="37" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="G5" s="38" t="s">
         <v>891</v>
@@ -8759,7 +8749,7 @@
       <c r="J5" s="102" t="s">
         <v>1222</v>
       </c>
-      <c r="K5" s="116" t="s">
+      <c r="K5" s="106" t="s">
         <v>890</v>
       </c>
       <c r="L5" s="40">
@@ -8786,7 +8776,7 @@
         <v>891</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="G6" s="21" t="s">
         <v>888</v>
@@ -8798,16 +8788,16 @@
         <v>893</v>
       </c>
       <c r="J6" s="103" t="s">
-        <v>1225</v>
-      </c>
-      <c r="K6" s="117" t="s">
+        <v>1223</v>
+      </c>
+      <c r="K6" s="107" t="s">
         <v>888</v>
       </c>
       <c r="L6" s="15">
         <v>0.1</v>
       </c>
       <c r="Q6" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
@@ -8827,7 +8817,7 @@
         <v>891</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="G7" s="21" t="s">
         <v>891</v>
@@ -8839,9 +8829,9 @@
         <v>893</v>
       </c>
       <c r="J7" s="103" t="s">
-        <v>1226</v>
-      </c>
-      <c r="K7" s="117" t="s">
+        <v>1222</v>
+      </c>
+      <c r="K7" s="107" t="s">
         <v>890</v>
       </c>
       <c r="L7" s="15">
@@ -8865,7 +8855,7 @@
         <v>888</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="G8" s="21" t="s">
         <v>891</v>
@@ -8877,9 +8867,9 @@
         <v>893</v>
       </c>
       <c r="J8" s="103" t="s">
-        <v>1225</v>
-      </c>
-      <c r="K8" s="117" t="s">
+        <v>1223</v>
+      </c>
+      <c r="K8" s="107" t="s">
         <v>888</v>
       </c>
       <c r="L8" s="15">
@@ -8903,7 +8893,7 @@
         <v>888</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="G9" s="21" t="s">
         <v>888</v>
@@ -8915,10 +8905,10 @@
         <v>893</v>
       </c>
       <c r="J9" s="103" t="s">
-        <v>1226</v>
-      </c>
-      <c r="K9" s="117" t="s">
-        <v>1363</v>
+        <v>1222</v>
+      </c>
+      <c r="K9" s="107" t="s">
+        <v>1361</v>
       </c>
       <c r="L9" s="15">
         <v>0.75</v>
@@ -8941,7 +8931,7 @@
         <v>891</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="G10" s="21" t="s">
         <v>888</v>
@@ -8953,9 +8943,9 @@
         <v>893</v>
       </c>
       <c r="J10" s="103" t="s">
-        <v>1225</v>
-      </c>
-      <c r="K10" s="117" t="s">
+        <v>1223</v>
+      </c>
+      <c r="K10" s="107" t="s">
         <v>891</v>
       </c>
       <c r="L10" s="15">
@@ -8973,7 +8963,7 @@
       <c r="H11" s="11"/>
       <c r="I11" s="13"/>
       <c r="J11" s="103"/>
-      <c r="K11" s="117"/>
+      <c r="K11" s="107"/>
       <c r="L11" s="15"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -8987,7 +8977,7 @@
       <c r="H12" s="11"/>
       <c r="I12" s="13"/>
       <c r="J12" s="103"/>
-      <c r="K12" s="117"/>
+      <c r="K12" s="107"/>
       <c r="L12" s="15"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -9001,7 +8991,7 @@
       <c r="H13" s="11"/>
       <c r="I13" s="13"/>
       <c r="J13" s="103"/>
-      <c r="K13" s="117"/>
+      <c r="K13" s="107"/>
       <c r="L13" s="15"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -9015,7 +9005,7 @@
       <c r="H14" s="11"/>
       <c r="I14" s="13"/>
       <c r="J14" s="103"/>
-      <c r="K14" s="117"/>
+      <c r="K14" s="107"/>
       <c r="L14" s="15"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -9029,7 +9019,7 @@
       <c r="H15" s="11"/>
       <c r="I15" s="13"/>
       <c r="J15" s="103"/>
-      <c r="K15" s="117"/>
+      <c r="K15" s="107"/>
       <c r="L15" s="15"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -9043,7 +9033,7 @@
       <c r="H16" s="11"/>
       <c r="I16" s="13"/>
       <c r="J16" s="103"/>
-      <c r="K16" s="117"/>
+      <c r="K16" s="107"/>
       <c r="L16" s="15"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -9057,7 +9047,7 @@
       <c r="H17" s="11"/>
       <c r="I17" s="13"/>
       <c r="J17" s="103"/>
-      <c r="K17" s="117"/>
+      <c r="K17" s="107"/>
       <c r="L17" s="15"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -9071,7 +9061,7 @@
       <c r="H18" s="11"/>
       <c r="I18" s="13"/>
       <c r="J18" s="103"/>
-      <c r="K18" s="117"/>
+      <c r="K18" s="107"/>
       <c r="L18" s="15"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -9085,7 +9075,7 @@
       <c r="H19" s="11"/>
       <c r="I19" s="13"/>
       <c r="J19" s="103"/>
-      <c r="K19" s="117"/>
+      <c r="K19" s="107"/>
       <c r="L19" s="15"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -9099,7 +9089,7 @@
       <c r="H20" s="11"/>
       <c r="I20" s="13"/>
       <c r="J20" s="103"/>
-      <c r="K20" s="117"/>
+      <c r="K20" s="107"/>
       <c r="L20" s="15"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -9113,7 +9103,7 @@
       <c r="H21" s="11"/>
       <c r="I21" s="13"/>
       <c r="J21" s="103"/>
-      <c r="K21" s="117"/>
+      <c r="K21" s="107"/>
       <c r="L21" s="15"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -9127,7 +9117,7 @@
       <c r="H22" s="11"/>
       <c r="I22" s="13"/>
       <c r="J22" s="103"/>
-      <c r="K22" s="117"/>
+      <c r="K22" s="107"/>
       <c r="L22" s="15"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -9141,7 +9131,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="13"/>
       <c r="J23" s="103"/>
-      <c r="K23" s="117"/>
+      <c r="K23" s="107"/>
       <c r="L23" s="15"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -9155,7 +9145,7 @@
       <c r="H24" s="11"/>
       <c r="I24" s="13"/>
       <c r="J24" s="103"/>
-      <c r="K24" s="117"/>
+      <c r="K24" s="107"/>
       <c r="L24" s="15"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -9169,7 +9159,7 @@
       <c r="H25" s="11"/>
       <c r="I25" s="13"/>
       <c r="J25" s="103"/>
-      <c r="K25" s="117"/>
+      <c r="K25" s="107"/>
       <c r="L25" s="15"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -9183,7 +9173,7 @@
       <c r="H26" s="11"/>
       <c r="I26" s="13"/>
       <c r="J26" s="103"/>
-      <c r="K26" s="117"/>
+      <c r="K26" s="107"/>
       <c r="L26" s="15"/>
     </row>
     <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9197,7 +9187,7 @@
       <c r="H27" s="12"/>
       <c r="I27" s="14"/>
       <c r="J27" s="104"/>
-      <c r="K27" s="118"/>
+      <c r="K27" s="108"/>
       <c r="L27" s="16"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -9344,121 +9334,121 @@
         <v>10</v>
       </c>
       <c r="K1" s="32" t="s">
+        <v>1230</v>
+      </c>
+      <c r="L1" s="32" t="s">
         <v>1232</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="M1" s="32" t="s">
         <v>1234</v>
       </c>
-      <c r="M1" s="32" t="s">
+      <c r="N1" s="32" t="s">
         <v>1236</v>
       </c>
-      <c r="N1" s="32" t="s">
+      <c r="O1" s="32" t="s">
         <v>1238</v>
       </c>
-      <c r="O1" s="32" t="s">
-        <v>1240</v>
-      </c>
       <c r="P1" s="32" t="s">
+        <v>1291</v>
+      </c>
+      <c r="Q1" s="32" t="s">
+        <v>1292</v>
+      </c>
+      <c r="R1" s="32" t="s">
         <v>1293</v>
       </c>
-      <c r="Q1" s="32" t="s">
+      <c r="S1" s="32" t="s">
+        <v>1295</v>
+      </c>
+      <c r="T1" s="32" t="s">
+        <v>1296</v>
+      </c>
+      <c r="U1" s="32" t="s">
+        <v>1297</v>
+      </c>
+      <c r="V1" s="32" t="s">
+        <v>1298</v>
+      </c>
+      <c r="W1" s="32" t="s">
+        <v>1299</v>
+      </c>
+      <c r="X1" s="32" t="s">
+        <v>1300</v>
+      </c>
+      <c r="Y1" s="32" t="s">
+        <v>1301</v>
+      </c>
+      <c r="Z1" s="32" t="s">
+        <v>1302</v>
+      </c>
+      <c r="AA1" s="32" t="s">
+        <v>1303</v>
+      </c>
+      <c r="AB1" s="32" t="s">
+        <v>1304</v>
+      </c>
+      <c r="AC1" s="32" t="s">
+        <v>1305</v>
+      </c>
+      <c r="AD1" s="32" t="s">
+        <v>1306</v>
+      </c>
+      <c r="AE1" s="32" t="s">
+        <v>1307</v>
+      </c>
+      <c r="AF1" s="32" t="s">
+        <v>1308</v>
+      </c>
+      <c r="AG1" s="32" t="s">
+        <v>1309</v>
+      </c>
+      <c r="AH1" s="32" t="s">
+        <v>1310</v>
+      </c>
+      <c r="AI1" s="32" t="s">
+        <v>1311</v>
+      </c>
+      <c r="AJ1" s="32" t="s">
+        <v>1312</v>
+      </c>
+      <c r="AK1" s="32" t="s">
+        <v>1313</v>
+      </c>
+      <c r="AL1" s="32" t="s">
         <v>1294</v>
       </c>
-      <c r="R1" s="32" t="s">
-        <v>1295</v>
-      </c>
-      <c r="S1" s="32" t="s">
-        <v>1297</v>
-      </c>
-      <c r="T1" s="32" t="s">
-        <v>1298</v>
-      </c>
-      <c r="U1" s="32" t="s">
-        <v>1299</v>
-      </c>
-      <c r="V1" s="32" t="s">
-        <v>1300</v>
-      </c>
-      <c r="W1" s="32" t="s">
-        <v>1301</v>
-      </c>
-      <c r="X1" s="32" t="s">
-        <v>1302</v>
-      </c>
-      <c r="Y1" s="32" t="s">
-        <v>1303</v>
-      </c>
-      <c r="Z1" s="32" t="s">
-        <v>1304</v>
-      </c>
-      <c r="AA1" s="32" t="s">
-        <v>1305</v>
-      </c>
-      <c r="AB1" s="32" t="s">
-        <v>1306</v>
-      </c>
-      <c r="AC1" s="32" t="s">
-        <v>1307</v>
-      </c>
-      <c r="AD1" s="32" t="s">
-        <v>1308</v>
-      </c>
-      <c r="AE1" s="32" t="s">
-        <v>1309</v>
-      </c>
-      <c r="AF1" s="32" t="s">
-        <v>1310</v>
-      </c>
-      <c r="AG1" s="32" t="s">
-        <v>1311</v>
-      </c>
-      <c r="AH1" s="32" t="s">
-        <v>1312</v>
-      </c>
-      <c r="AI1" s="32" t="s">
-        <v>1313</v>
-      </c>
-      <c r="AJ1" s="32" t="s">
+      <c r="AM1" s="32" t="s">
+        <v>1261</v>
+      </c>
+      <c r="AN1" s="32" t="s">
+        <v>1263</v>
+      </c>
+      <c r="AO1" s="32" t="s">
+        <v>1265</v>
+      </c>
+      <c r="AP1" s="32" t="s">
+        <v>1267</v>
+      </c>
+      <c r="AQ1" s="32" t="s">
+        <v>1269</v>
+      </c>
+      <c r="AR1" s="32" t="s">
+        <v>1271</v>
+      </c>
+      <c r="AS1" s="32" t="s">
         <v>1314</v>
       </c>
-      <c r="AK1" s="32" t="s">
-        <v>1315</v>
-      </c>
-      <c r="AL1" s="32" t="s">
-        <v>1296</v>
-      </c>
-      <c r="AM1" s="32" t="s">
-        <v>1263</v>
-      </c>
-      <c r="AN1" s="32" t="s">
-        <v>1265</v>
-      </c>
-      <c r="AO1" s="32" t="s">
-        <v>1267</v>
-      </c>
-      <c r="AP1" s="32" t="s">
-        <v>1269</v>
-      </c>
-      <c r="AQ1" s="32" t="s">
-        <v>1271</v>
-      </c>
-      <c r="AR1" s="32" t="s">
-        <v>1273</v>
-      </c>
-      <c r="AS1" s="32" t="s">
-        <v>1316</v>
-      </c>
       <c r="AT1" s="32" t="s">
+        <v>1274</v>
+      </c>
+      <c r="AU1" s="32" t="s">
         <v>1276</v>
       </c>
-      <c r="AU1" s="32" t="s">
+      <c r="AV1" s="32" t="s">
         <v>1278</v>
       </c>
-      <c r="AV1" s="32" t="s">
+      <c r="AW1" s="32" t="s">
         <v>1280</v>
-      </c>
-      <c r="AW1" s="32" t="s">
-        <v>1282</v>
       </c>
       <c r="AX1" s="32" t="s">
         <v>49</v>
@@ -81803,11 +81793,11 @@
         <f>IF(C2="", "", 1.28*SQRT((D2*(1-D2))/$J$2))</f>
         <v>3.9508701573197767E-2</v>
       </c>
-      <c r="G2" s="111" t="s">
+      <c r="G2" s="115" t="s">
         <v>1205</v>
       </c>
-      <c r="H2" s="112"/>
-      <c r="I2" s="112"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="116"/>
       <c r="J2" s="59">
         <f>COUNT('TerrADat Data Dump'!A1:A1000)</f>
         <v>256</v>
@@ -82404,10 +82394,10 @@
         <f>IF(A2="", "", 1.28*SQRT((D2*(1-D2))/$I$2))</f>
         <v>#N/A</v>
       </c>
-      <c r="G2" s="113" t="s">
+      <c r="G2" s="117" t="s">
         <v>1204</v>
       </c>
-      <c r="H2" s="114"/>
+      <c r="H2" s="118"/>
       <c r="I2" s="62">
         <f>COUNT('LMF Data Dump'!A2:A1000)</f>
         <v>211</v>
@@ -82971,725 +82961,725 @@
         <v>897</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="B2" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="C2" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
       <c r="B3" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="C3" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="B4" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="C4" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="B5" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="C5" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="B6" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="C6" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="B7" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="C7" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="B8" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="C8" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="B9" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="C9" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="B10" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="C10" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="B11" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
       <c r="C11" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="B12" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
       <c r="C12" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="B13" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
       <c r="C13" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="B14" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="C14" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="B15" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
       <c r="C15" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="B16" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="C16" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="B17" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="C17" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="B18" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="C18" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="B19" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
       <c r="C19" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="B20" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
       <c r="C20" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
       <c r="B21" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
       <c r="C21" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="B22" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
       <c r="C22" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="B23" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
       <c r="C23" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="B24" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
       <c r="C24" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="B25" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
       <c r="C25" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="B26" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
       <c r="C26" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="B27" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="C27" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="B28" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="C28" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="B29" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="C29" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="B30" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
       <c r="C30" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="B31" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="C31" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="B32" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="C32" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="B33" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="C33" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="B34" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="C34" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="B35" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="C35" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="B36" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="C36" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="B37" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="C37" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="B38" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="C38" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="B39" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
       <c r="C39" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
       <c r="B40" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
       <c r="C40" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
       <c r="B41" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
       <c r="C41" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
       <c r="B42" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="C42" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="B43" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="C43" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="B44" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
       <c r="C44" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="B45" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="C45" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="B46" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="C46" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="B47" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
       <c r="C47" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
       <c r="B48" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="C48" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="B49" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="C49" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="B50" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="C50" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="B51" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="C51" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="B52" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="C52" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
       <c r="B53" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="C53" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
       <c r="B54" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="C54" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="B55" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="C55" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="B56" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="C56" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
       <c r="B57" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="C57" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="B58" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="C58" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
       <c r="B59" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
       <c r="C59" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="B60" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
       <c r="C60" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="B61" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="C61" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="B62" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="C62" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="B63" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="C63" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="B64" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
       <c r="C64" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
       <c r="B65" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
       <c r="C65" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
       <c r="B66" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
       <c r="C66" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Grunt work and reorginzation
</commit_message>
<xml_diff>
--- a/benchmarking/TerrestrialAIM_DataAnalysis_Template.xlsx
+++ b/benchmarking/TerrestrialAIM_DataAnalysis_Template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4070" uniqueCount="1363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4070" uniqueCount="1365">
   <si>
     <t>Management Question</t>
   </si>
@@ -4349,6 +4349,12 @@
   </si>
   <si>
     <t>Proportion Relation</t>
+  </si>
+  <si>
+    <t>Not meeting</t>
+  </si>
+  <si>
+    <t>Meeting</t>
   </si>
 </sst>
 </file>
@@ -8521,7 +8527,7 @@
   <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8788,7 +8794,7 @@
         <v>893</v>
       </c>
       <c r="J6" s="103" t="s">
-        <v>1223</v>
+        <v>1363</v>
       </c>
       <c r="K6" s="107" t="s">
         <v>888</v>
@@ -8829,7 +8835,7 @@
         <v>893</v>
       </c>
       <c r="J7" s="103" t="s">
-        <v>1222</v>
+        <v>1364</v>
       </c>
       <c r="K7" s="107" t="s">
         <v>890</v>
@@ -8867,7 +8873,7 @@
         <v>893</v>
       </c>
       <c r="J8" s="103" t="s">
-        <v>1223</v>
+        <v>1363</v>
       </c>
       <c r="K8" s="107" t="s">
         <v>888</v>
@@ -8905,7 +8911,7 @@
         <v>893</v>
       </c>
       <c r="J9" s="103" t="s">
-        <v>1222</v>
+        <v>1364</v>
       </c>
       <c r="K9" s="107" t="s">
         <v>1361</v>
@@ -8943,7 +8949,7 @@
         <v>893</v>
       </c>
       <c r="J10" s="103" t="s">
-        <v>1223</v>
+        <v>1363</v>
       </c>
       <c r="K10" s="107" t="s">
         <v>891</v>

</xml_diff>